<commit_message>
Moved in loose assets from other directories.
</commit_message>
<xml_diff>
--- a/Work/IngredientsBuffs.xlsx
+++ b/Work/IngredientsBuffs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Dev\Projects\SDV\Projects\CooksAssistant\Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02154EE-19EE-4D51-9B26-B5BB9664C1AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1AC63D3-A4E7-4B70-95CF-38C7EA66929D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8745" yWindow="10335" windowWidth="26310" windowHeight="12720" xr2:uid="{5C123163-A56D-4F33-9D03-6A7D31F84288}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="79">
   <si>
     <t>FORAGING</t>
   </si>
@@ -261,6 +261,15 @@
   </si>
   <si>
     <t>Spring Onion</t>
+  </si>
+  <si>
+    <t>Cranberry Sauce</t>
+  </si>
+  <si>
+    <t>Stuffing</t>
+  </si>
+  <si>
+    <t>Pancakes</t>
   </si>
 </sst>
 </file>
@@ -685,7 +694,7 @@
   <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -734,7 +743,7 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>54</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>41</v>
@@ -771,8 +780,8 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>54</v>
+      <c r="A3" s="3" t="s">
+        <v>38</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>75</v>
@@ -810,7 +819,7 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>36</v>
@@ -853,6 +862,9 @@
       <c r="C5" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="D5" s="3" t="s">
+        <v>77</v>
+      </c>
       <c r="F5" s="2" t="s">
         <v>47</v>
       </c>
@@ -865,8 +877,8 @@
       <c r="I5" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="J5" s="4" t="s">
-        <v>40</v>
+      <c r="J5" s="3" t="s">
+        <v>78</v>
       </c>
       <c r="L5" s="2" t="s">
         <v>60</v>
@@ -888,6 +900,9 @@
       <c r="I6" s="6" t="s">
         <v>44</v>
       </c>
+      <c r="J6" s="4" t="s">
+        <v>76</v>
+      </c>
       <c r="L6" s="2" t="s">
         <v>64</v>
       </c>
@@ -904,6 +919,9 @@
       </c>
       <c r="H7" s="4" t="s">
         <v>43</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="L7" s="2" t="s">
         <v>62</v>

</xml_diff>